<commit_message>
upload readme yiuyeung ng
</commit_message>
<xml_diff>
--- a/Project Management/Time sheet/Timetsheet - Ng Yiu Yeung.xlsx
+++ b/Project Management/Time sheet/Timetsheet - Ng Yiu Yeung.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Desktop/MCI_2021/MCI_Project/Team-024/Agenda_Minutes_Timesheet/Time sheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Desktop/MCI_2021/MCI_Project/Team-024/Project Management/Time sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38FC220-EAEE-9D4B-8E76-A48C66FACBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9112D305-C6D0-0849-BF91-3084543FB1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="500" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29700" windowHeight="17360" tabRatio="500" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 2 " sheetId="3" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Week 9" sheetId="17" r:id="rId10"/>
     <sheet name="Week 10" sheetId="19" r:id="rId11"/>
     <sheet name="Week 11" sheetId="21" r:id="rId12"/>
+    <sheet name="Week 12" sheetId="23" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Week 2 '!$A$1:$H$13</definedName>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="116">
   <si>
     <t>MCI Project Weekly Time Sheet</t>
   </si>
@@ -392,6 +393,18 @@
   </si>
   <si>
     <t>Demo presentation</t>
+  </si>
+  <si>
+    <t>Poster review</t>
+  </si>
+  <si>
+    <t>Demo preparation</t>
+  </si>
+  <si>
+    <t>Final Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Report </t>
   </si>
 </sst>
 </file>
@@ -584,7 +597,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -675,6 +688,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1022,7 +1038,7 @@
   <dimension ref="A2:AW12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1106,7 +1122,9 @@
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="33">
+        <v>44263</v>
+      </c>
       <c r="C6" s="18">
         <v>0.58333333333333337</v>
       </c>
@@ -1171,7 +1189,9 @@
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="33">
+        <v>44264</v>
+      </c>
       <c r="C7" s="17">
         <v>0.58333333333333337</v>
       </c>
@@ -1236,7 +1256,9 @@
       <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="33">
+        <v>44265</v>
+      </c>
       <c r="C8" s="17">
         <v>0.41666666666666669</v>
       </c>
@@ -1301,7 +1323,9 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="33">
+        <v>44266</v>
+      </c>
       <c r="C9" s="18">
         <v>0.375</v>
       </c>
@@ -1366,7 +1390,9 @@
       <c r="A10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="33">
+        <v>44267</v>
+      </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
@@ -1419,7 +1445,9 @@
       <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="33">
+        <v>44268</v>
+      </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="12"/>
@@ -1502,8 +1530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5C769E-887C-E449-9359-E94C29568739}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1542,7 +1570,7 @@
         <v>3</v>
       </c>
       <c r="H2">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -1575,7 +1603,9 @@
       <c r="A5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="33">
+        <v>44326</v>
+      </c>
       <c r="C5" s="21">
         <v>0.375</v>
       </c>
@@ -1599,7 +1629,9 @@
       <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="33">
+        <v>44327</v>
+      </c>
       <c r="C6" s="17">
         <v>0.58333333333333337</v>
       </c>
@@ -1619,11 +1651,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="33">
+        <v>44328</v>
+      </c>
       <c r="C7" s="17">
         <v>0.45833333333333331</v>
       </c>
@@ -1643,11 +1677,13 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="33">
+        <v>44329</v>
+      </c>
       <c r="C8" s="23">
         <v>0.41666666666666669</v>
       </c>
@@ -1671,7 +1707,9 @@
       <c r="A9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="33">
+        <v>44330</v>
+      </c>
       <c r="C9" s="23">
         <v>0.45833333333333331</v>
       </c>
@@ -1695,7 +1733,9 @@
       <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="33">
+        <v>44331</v>
+      </c>
       <c r="C10" s="21">
         <v>0.625</v>
       </c>
@@ -1742,8 +1782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D0C30A-14AB-9C4F-9B2C-C55D45EFCF76}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1782,7 +1822,7 @@
         <v>3</v>
       </c>
       <c r="H2">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -1815,7 +1855,9 @@
       <c r="A5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="33">
+        <v>44333</v>
+      </c>
       <c r="C5" s="21">
         <v>0.375</v>
       </c>
@@ -1839,7 +1881,9 @@
       <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="33">
+        <v>44334</v>
+      </c>
       <c r="C6" s="17">
         <v>0.58333333333333337</v>
       </c>
@@ -1855,7 +1899,9 @@
       <c r="A7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="33">
+        <v>44335</v>
+      </c>
       <c r="C7" s="17">
         <v>0.375</v>
       </c>
@@ -1879,7 +1925,9 @@
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="33">
+        <v>44336</v>
+      </c>
       <c r="C8" s="23">
         <v>0.41666666666666669</v>
       </c>
@@ -1903,7 +1951,9 @@
       <c r="A9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="33">
+        <v>44337</v>
+      </c>
       <c r="C9" s="23">
         <v>0.45833333333333331</v>
       </c>
@@ -1925,7 +1975,9 @@
     </row>
     <row r="10" spans="1:8" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+      <c r="B10" s="33">
+        <v>44338</v>
+      </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
       <c r="E10" s="12"/>
@@ -1960,8 +2012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C09D32-7617-0244-BCB3-9A075460CE35}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2000,7 +2052,7 @@
         <v>3</v>
       </c>
       <c r="H2">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -2033,7 +2085,9 @@
       <c r="A5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="33">
+        <v>44340</v>
+      </c>
       <c r="C5" s="21">
         <v>0.375</v>
       </c>
@@ -2057,7 +2111,9 @@
       <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="33">
+        <v>44341</v>
+      </c>
       <c r="C6" s="17">
         <v>0.58333333333333337</v>
       </c>
@@ -2081,7 +2137,9 @@
       <c r="A7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="33">
+        <v>44342</v>
+      </c>
       <c r="C7" s="17">
         <v>0.45833333333333331</v>
       </c>
@@ -2105,7 +2163,9 @@
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="33">
+        <v>44343</v>
+      </c>
       <c r="C8" s="23">
         <v>0.41666666666666669</v>
       </c>
@@ -2129,7 +2189,9 @@
       <c r="A9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="33">
+        <v>44344</v>
+      </c>
       <c r="C9" s="23">
         <v>0.70833333333333337</v>
       </c>
@@ -2153,7 +2215,9 @@
       <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="33">
+        <v>44345</v>
+      </c>
       <c r="C10" s="21">
         <v>0.66666666666666663</v>
       </c>
@@ -2188,6 +2252,258 @@
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C5:D10" xr:uid="{1A58267C-DF13-F14F-B767-042AC4CFE1EC}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C548354E-5442-EE42-B4E6-3430E2153C89}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="46.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="33">
+        <v>44347</v>
+      </c>
+      <c r="C5" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="D5" s="21">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E5" s="12">
+        <v>2</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="33">
+        <v>44348</v>
+      </c>
+      <c r="C6" s="17">
+        <v>0.625</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E6" s="12">
+        <v>4</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="33">
+        <v>44349</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0.625</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="12">
+        <v>3</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="33">
+        <v>44350</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E8" s="12">
+        <v>5</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="33">
+        <v>44351</v>
+      </c>
+      <c r="C9" s="23">
+        <v>0.375</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E9" s="12">
+        <v>2</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="33">
+        <v>44352</v>
+      </c>
+      <c r="C10" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="21">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E10" s="12">
+        <v>5</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="8">
+        <f>SUM(E5:E10)</f>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C5:D10" xr:uid="{2EF5F773-CDC4-5248-B883-CC6BC2559A06}">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>
@@ -2204,7 +2520,7 @@
   <dimension ref="A2:AW12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2288,7 +2604,9 @@
       <c r="A6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="33">
+        <v>44270</v>
+      </c>
       <c r="C6" s="21">
         <v>0.5</v>
       </c>
@@ -2353,7 +2671,9 @@
       <c r="A7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="33">
+        <v>44271</v>
+      </c>
       <c r="C7" s="23">
         <v>0.41666666666666669</v>
       </c>
@@ -2418,7 +2738,9 @@
       <c r="A8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="33">
+        <v>44272</v>
+      </c>
       <c r="C8" s="24">
         <v>0.375</v>
       </c>
@@ -2483,7 +2805,9 @@
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="33">
+        <v>44273</v>
+      </c>
       <c r="C9" s="23">
         <v>0.375</v>
       </c>
@@ -2548,7 +2872,9 @@
       <c r="A10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="33">
+        <v>44274</v>
+      </c>
       <c r="C10" s="21">
         <v>0.66666666666666663</v>
       </c>
@@ -2613,7 +2939,9 @@
       <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="33">
+        <v>44275</v>
+      </c>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="E11" s="12"/>
@@ -2701,7 +3029,7 @@
   <dimension ref="A2:AW12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2785,7 +3113,9 @@
       <c r="A6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="33">
+        <v>44277</v>
+      </c>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="12"/>
@@ -2838,7 +3168,9 @@
       <c r="A7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="33">
+        <v>44278</v>
+      </c>
       <c r="C7" s="21">
         <v>0.375</v>
       </c>
@@ -2903,7 +3235,9 @@
       <c r="A8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="33">
+        <v>44279</v>
+      </c>
       <c r="C8" s="23">
         <v>0.375</v>
       </c>
@@ -2968,7 +3302,9 @@
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="33">
+        <v>44280</v>
+      </c>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="12"/>
@@ -3021,7 +3357,9 @@
       <c r="A10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="33">
+        <v>44281</v>
+      </c>
       <c r="C10" s="21">
         <v>0.66666666666666663</v>
       </c>
@@ -3086,7 +3424,9 @@
       <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="33">
+        <v>44282</v>
+      </c>
       <c r="C11" s="23">
         <v>0.60416666666666663</v>
       </c>
@@ -3185,7 +3525,7 @@
   <dimension ref="A2:AW12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B6" sqref="B6:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3312,7 +3652,9 @@
       <c r="A6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="33">
+        <v>44284</v>
+      </c>
       <c r="C6" s="21">
         <v>0.375</v>
       </c>
@@ -3377,7 +3719,9 @@
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="33">
+        <v>44285</v>
+      </c>
       <c r="C7" s="17">
         <v>0.58333333333333337</v>
       </c>
@@ -3442,7 +3786,9 @@
       <c r="A8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="33">
+        <v>44286</v>
+      </c>
       <c r="C8" s="23">
         <v>0.41666666666666669</v>
       </c>
@@ -3507,7 +3853,9 @@
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="33">
+        <v>44287</v>
+      </c>
       <c r="C9" s="23">
         <v>0.75</v>
       </c>
@@ -3572,7 +3920,9 @@
       <c r="A10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="33">
+        <v>44288</v>
+      </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
       <c r="E10" s="12"/>
@@ -3625,7 +3975,9 @@
       <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="33">
+        <v>44289</v>
+      </c>
       <c r="C11" s="21">
         <v>0.45833333333333331</v>
       </c>
@@ -3679,8 +4031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E57F0CE-B4FB-2848-8FF7-4DF110FCC13C}">
   <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3748,11 +4100,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="33">
+        <v>44291</v>
+      </c>
       <c r="C6" s="21">
         <v>0.375</v>
       </c>
@@ -3772,11 +4126,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="33">
+        <v>44292</v>
+      </c>
       <c r="C7" s="17">
         <v>0.58333333333333337</v>
       </c>
@@ -3796,11 +4152,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="33">
+        <v>44293</v>
+      </c>
       <c r="C8" s="23">
         <v>0.45833333333333331</v>
       </c>
@@ -3820,11 +4178,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="33">
+        <v>44294</v>
+      </c>
       <c r="C9" s="23">
         <v>0.41666666666666669</v>
       </c>
@@ -3848,7 +4208,9 @@
       <c r="A10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="33">
+        <v>44295</v>
+      </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
       <c r="E10" s="12"/>
@@ -3860,7 +4222,9 @@
       <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="33">
+        <v>44296</v>
+      </c>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
       <c r="E11" s="12"/>
@@ -3896,7 +4260,7 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B6" sqref="B6:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3964,11 +4328,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="33">
+        <v>44298</v>
+      </c>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="12"/>
@@ -3976,11 +4342,13 @@
       <c r="G6" s="22"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="33">
+        <v>44299</v>
+      </c>
       <c r="C7" s="17">
         <v>0.58333333333333337</v>
       </c>
@@ -4000,11 +4368,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="33">
+        <v>44300</v>
+      </c>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
       <c r="E8" s="12"/>
@@ -4016,7 +4386,9 @@
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="33">
+        <v>44301</v>
+      </c>
       <c r="C9" s="23">
         <v>0.41666666666666669</v>
       </c>
@@ -4036,11 +4408,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="33">
+        <v>44302</v>
+      </c>
       <c r="C10" s="23">
         <v>0.45833333333333331</v>
       </c>
@@ -4060,11 +4434,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="82" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="33">
+        <v>44303</v>
+      </c>
       <c r="C11" s="21">
         <v>0.54166666666666663</v>
       </c>
@@ -4111,8 +4487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A492DFD-6522-0A44-A5A1-C7AD6BB3DFF5}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4151,7 +4527,7 @@
         <v>3</v>
       </c>
       <c r="H2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -4184,7 +4560,9 @@
       <c r="A5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="33">
+        <v>44305</v>
+      </c>
       <c r="C5" s="21">
         <v>0.375</v>
       </c>
@@ -4208,7 +4586,9 @@
       <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="33">
+        <v>44306</v>
+      </c>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="12"/>
@@ -4220,7 +4600,9 @@
       <c r="A7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="33">
+        <v>44307</v>
+      </c>
       <c r="C7" s="17">
         <v>0.45833333333333331</v>
       </c>
@@ -4244,7 +4626,9 @@
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="33">
+        <v>44308</v>
+      </c>
       <c r="C8" s="23">
         <v>0.41666666666666669</v>
       </c>
@@ -4268,7 +4652,9 @@
       <c r="A9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="33">
+        <v>44309</v>
+      </c>
       <c r="C9" s="23">
         <v>0.45833333333333331</v>
       </c>
@@ -4292,7 +4678,9 @@
       <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="33">
+        <v>44310</v>
+      </c>
       <c r="C10" s="21">
         <v>0.58333333333333337</v>
       </c>
@@ -4340,7 +4728,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4379,7 +4767,7 @@
         <v>3</v>
       </c>
       <c r="H2">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4412,7 +4800,9 @@
       <c r="A5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="33">
+        <v>44312</v>
+      </c>
       <c r="C5" s="21">
         <v>0.375</v>
       </c>
@@ -4436,7 +4826,9 @@
       <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="33">
+        <v>44313</v>
+      </c>
       <c r="C6" s="17">
         <v>0.58333333333333337</v>
       </c>
@@ -4460,7 +4852,9 @@
       <c r="A7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="33">
+        <v>44314</v>
+      </c>
       <c r="C7" s="17">
         <v>0.41666666666666669</v>
       </c>
@@ -4484,7 +4878,9 @@
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="33">
+        <v>44315</v>
+      </c>
       <c r="C8" s="23">
         <v>0.41666666666666669</v>
       </c>
@@ -4508,7 +4904,9 @@
       <c r="A9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="33">
+        <v>44316</v>
+      </c>
       <c r="C9" s="23">
         <v>0.45833333333333331</v>
       </c>
@@ -4532,7 +4930,9 @@
       <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="33">
+        <v>44317</v>
+      </c>
       <c r="C10" s="21">
         <v>0.58333333333333337</v>
       </c>
@@ -4580,7 +4980,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:H6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4619,7 +5019,7 @@
         <v>3</v>
       </c>
       <c r="H2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4652,7 +5052,9 @@
       <c r="A5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="33">
+        <v>44319</v>
+      </c>
       <c r="C5" s="21">
         <v>0.5</v>
       </c>
@@ -4676,7 +5078,9 @@
       <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="33">
+        <v>44320</v>
+      </c>
       <c r="C6" s="17">
         <v>0.58333333333333337</v>
       </c>
@@ -4700,7 +5104,9 @@
       <c r="A7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="33">
+        <v>44321</v>
+      </c>
       <c r="C7" s="17">
         <v>0.45833333333333331</v>
       </c>
@@ -4724,7 +5130,9 @@
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="33">
+        <v>44322</v>
+      </c>
       <c r="C8" s="23">
         <v>0.41666666666666669</v>
       </c>
@@ -4748,7 +5156,9 @@
       <c r="A9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="33">
+        <v>44323</v>
+      </c>
       <c r="C9" s="23">
         <v>0.45833333333333331</v>
       </c>
@@ -4772,7 +5182,9 @@
       <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="33">
+        <v>44324</v>
+      </c>
       <c r="C10" s="21">
         <v>0.625</v>
       </c>

</xml_diff>